<commit_message>
feat : opi->esp 패킷 파싱
</commit_message>
<xml_diff>
--- a/docs/프로토콜.xlsx
+++ b/docs/프로토콜.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mju-my.sharepoint.com/personal/sleepy1001_mju_ac_kr/Documents/학교/2023-2/융캡2/MyongJa_FW/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="8_{A837F3A6-F922-48FF-99B8-8166A3865843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68D99FD6-85DE-4C17-B7AD-A2348167F52D}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="8_{A837F3A6-F922-48FF-99B8-8166A3865843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4E8E719-C91F-49A9-9960-9A9A9AFAB3CE}"/>
   <bookViews>
-    <workbookView xWindow="2085" yWindow="3105" windowWidth="22695" windowHeight="15285" xr2:uid="{11071A3E-6F36-4C24-93C4-F6C00B063016}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{11071A3E-6F36-4C24-93C4-F6C00B063016}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="48">
   <si>
     <t>SOF</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -219,6 +219,14 @@
   </si>
   <si>
     <t>]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>o -&gt; e</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>e -&gt; o</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -596,20 +604,20 @@
   <dimension ref="D4:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="8.625" customWidth="1"/>
-    <col min="4" max="7" width="10.625" customWidth="1"/>
+    <col min="3" max="3" width="8.58203125" customWidth="1"/>
+    <col min="4" max="7" width="10.58203125" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
-    <col min="10" max="10" width="13.375" customWidth="1"/>
-    <col min="11" max="11" width="28.875" customWidth="1"/>
-    <col min="12" max="12" width="9.375" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" customWidth="1"/>
+    <col min="11" max="11" width="28.83203125" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="4:12" x14ac:dyDescent="0.45">
       <c r="D4" t="s">
         <v>5</v>
       </c>
@@ -620,7 +628,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:12" x14ac:dyDescent="0.45">
       <c r="D5" t="s">
         <v>6</v>
       </c>
@@ -628,7 +636,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:12" x14ac:dyDescent="0.45">
       <c r="D6" t="s">
         <v>10</v>
       </c>
@@ -636,7 +644,10 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:12" x14ac:dyDescent="0.45">
+      <c r="D9" t="s">
+        <v>46</v>
+      </c>
       <c r="F9" t="s">
         <v>0</v>
       </c>
@@ -659,7 +670,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
         <v>44</v>
@@ -683,7 +694,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
         <v>44</v>
@@ -707,8 +718,11 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="13" spans="4:12" x14ac:dyDescent="0.45">
+      <c r="D13" t="s">
+        <v>47</v>
+      </c>
       <c r="F13" t="s">
         <v>0</v>
       </c>
@@ -731,7 +745,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
         <v>34</v>
@@ -755,7 +769,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E15" s="1"/>
       <c r="F15" s="1" t="s">
         <v>34</v>
@@ -779,7 +793,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
         <v>34</v>
@@ -803,7 +817,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:12" x14ac:dyDescent="0.45">
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
         <v>34</v>
@@ -827,7 +841,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:12" x14ac:dyDescent="0.45">
       <c r="G19" t="s">
         <v>0</v>
       </c>
@@ -844,7 +858,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:12" x14ac:dyDescent="0.45">
       <c r="G20" s="1" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
feat : esp-opi 패킷 전송 함수
</commit_message>
<xml_diff>
--- a/docs/프로토콜.xlsx
+++ b/docs/프로토콜.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mju-my.sharepoint.com/personal/sleepy1001_mju_ac_kr/Documents/학교/2023-2/융캡2/MyongJa_FW/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="8_{A837F3A6-F922-48FF-99B8-8166A3865843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4E8E719-C91F-49A9-9960-9A9A9AFAB3CE}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="8_{A837F3A6-F922-48FF-99B8-8166A3865843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1EDE5397-53BE-4558-824F-1C1A113CCD66}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{11071A3E-6F36-4C24-93C4-F6C00B063016}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="49">
   <si>
     <t>SOF</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -227,6 +227,10 @@
   </si>
   <si>
     <t>e -&gt; o</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1초</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -604,7 +608,7 @@
   <dimension ref="D4:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -790,7 +794,7 @@
         <v>22</v>
       </c>
       <c r="L15" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="4:12" x14ac:dyDescent="0.45">
@@ -838,7 +842,7 @@
         <v>25</v>
       </c>
       <c r="L17" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="5:12" x14ac:dyDescent="0.45">

</xml_diff>